<commit_message>
creates the authors and books with a route
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Training Projects\Books\Task\2nd Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahesty.nasser\Desktop\Tasks\Book-Adding\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="518">
   <si>
     <t>Iure voluptates et facere reprehenderit nobis autem</t>
   </si>
@@ -1568,6 +1568,12 @@
   </si>
   <si>
     <t>author_name</t>
+  </si>
+  <si>
+    <t>grtg</t>
+  </si>
+  <si>
+    <t>iuyiryuk</t>
   </si>
 </sst>
 </file>
@@ -1622,8 +1628,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H101" totalsRowShown="0">
-  <autoFilter ref="A1:H101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H102" totalsRowShown="0">
+  <autoFilter ref="A1:H102"/>
   <tableColumns count="8">
     <tableColumn id="1" name="title"/>
     <tableColumn id="2" name="author"/>
@@ -1935,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4583,6 +4589,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>517</v>
+      </c>
+      <c r="C102" t="s">
+        <v>516</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <tableParts count="1">
@@ -4595,7 +4609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added some error handling
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="518">
   <si>
     <t>Iure voluptates et facere reprehenderit nobis autem</t>
   </si>
@@ -1573,7 +1573,7 @@
     <t>grtg</t>
   </si>
   <si>
-    <t>iuyiryuk</t>
+    <t>jkhdcsgkf</t>
   </si>
 </sst>
 </file>
@@ -1943,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="B85" workbookViewId="0">
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4593,8 +4593,14 @@
       <c r="A102" t="s">
         <v>517</v>
       </c>
+      <c r="B102" t="s">
+        <v>44</v>
+      </c>
       <c r="C102" t="s">
         <v>516</v>
+      </c>
+      <c r="H102" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>